<commit_message>
Initial Managment report section
</commit_message>
<xml_diff>
--- a/Thematic-Coding-Analysis-Tool.xlsx
+++ b/Thematic-Coding-Analysis-Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\Dropbox\Kieran Third year\BCIS301 _ AMIC700\Assignment 1\BCIS301---AMIC700---Thematic-Coding-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335E3877-1ED0-42C9-B72B-5DA7DB61CBF1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93C82FC-001D-4FBD-A494-5FE16CB1582E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="416">
   <si>
     <t>Extract</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1290,21 +1290,6 @@
 Team and Audit and Assurance Committee, and the weaknesses in the project’s governance, 6 Executive Summary are matters for which a Chief Executive must take accountability</t>
   </si>
   <si>
-    <t>Open Communication Policy</t>
-  </si>
-  <si>
-    <t>Project Closure Policy</t>
-  </si>
-  <si>
-    <t>Crucial project momentum </t>
-  </si>
-  <si>
-    <t>Team dynamics</t>
-  </si>
-  <si>
-    <t>Comprehensive planning </t>
-  </si>
-  <si>
     <t>Risk Analysis</t>
   </si>
   <si>
@@ -1469,6 +1454,24 @@
   </si>
   <si>
     <t xml:space="preserve">In some cases the IT systems were not capable of producing information used to record the immunisation status, or monitor the immunisation side-effects among children (PAC, 2007). This contributed to delays in providing vaccinations to children; one report claimed that up to 3,000 children were not up-to-date with their vaccinations (Revel, 2006). </t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Deliverable</t>
+  </si>
+  <si>
+    <t>Management</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1848,9 +1851,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1866,7 +1866,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1876,7 +1884,13 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1885,13 +1899,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3354,12 +3362,12 @@
   </sortState>
   <tableColumns count="7">
     <tableColumn id="9" xr3:uid="{40CD8F54-5D7D-4314-8086-F0C4E8CE116C}" name="Ref" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{F0ECC283-9151-4B62-A20D-99F7825349D0}" name="Case Study" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9F9E6DB9-0D32-4F05-BFF0-DB43451BF75C}" name="Extract" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{DF84868F-687C-48AF-A90C-43543DC8CB0A}" name="Location" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B8DD23A4-B58B-4653-AE3F-31948D216593}" name="Summary" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{427DC161-A0D9-41D9-A494-C3575733222B}" name="Code" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{68C072C1-5BCD-4A05-B3ED-01263C1BAD6B}" name="Supergroup" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{F0ECC283-9151-4B62-A20D-99F7825349D0}" name="Case Study" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9F9E6DB9-0D32-4F05-BFF0-DB43451BF75C}" name="Extract" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DF84868F-687C-48AF-A90C-43543DC8CB0A}" name="Location" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B8DD23A4-B58B-4653-AE3F-31948D216593}" name="Summary" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{427DC161-A0D9-41D9-A494-C3575733222B}" name="Code" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{68C072C1-5BCD-4A05-B3ED-01263C1BAD6B}" name="Supergroup" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3631,8 +3639,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3654,7 +3662,7 @@
         <v>341</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -3669,20 +3677,20 @@
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A2" s="45">
+      <c r="A2" s="44">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="42" t="s">
         <v>218</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -3693,16 +3701,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A3" s="45">
+      <c r="A3" s="44">
         <v>2</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>400</v>
-      </c>
-      <c r="E3" s="43"/>
+      <c r="C3" s="43" t="s">
+        <v>395</v>
+      </c>
+      <c r="E3" s="42"/>
       <c r="F3" s="6" t="s">
         <v>293</v>
       </c>
@@ -3711,16 +3719,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A4" s="45">
+      <c r="A4" s="44">
         <v>3</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="6" t="s">
         <v>293</v>
       </c>
@@ -3729,16 +3737,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A5" s="45">
+      <c r="A5" s="44">
         <v>4</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>401</v>
-      </c>
-      <c r="E5" s="43" t="s">
+      <c r="C5" s="43" t="s">
+        <v>396</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>319</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -3749,19 +3757,19 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A6" s="45">
+      <c r="A6" s="44">
         <v>5</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>402</v>
+      <c r="C6" s="43" t="s">
+        <v>397</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="42" t="s">
         <v>81</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -3772,19 +3780,19 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A7" s="45">
+      <c r="A7" s="44">
         <v>6</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>325</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="42" t="s">
         <v>327</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -3795,19 +3803,19 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A8" s="45">
+      <c r="A8" s="44">
         <v>7</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="42" t="s">
         <v>244</v>
       </c>
       <c r="F8" s="10" t="s">
@@ -3818,16 +3826,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A9" s="45">
+      <c r="A9" s="44">
         <v>8</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="42" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -3838,16 +3846,16 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A10" s="45">
+      <c r="A10" s="44">
         <v>9</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>403</v>
-      </c>
-      <c r="E10" s="43" t="s">
+      <c r="C10" s="43" t="s">
+        <v>398</v>
+      </c>
+      <c r="E10" s="42" t="s">
         <v>247</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -3858,17 +3866,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A11" s="45">
+      <c r="A11" s="44">
         <v>10</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="43" t="s">
-        <v>404</v>
+      <c r="E11" s="42" t="s">
+        <v>399</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>296</v>
@@ -3878,16 +3886,16 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A12" s="45">
+      <c r="A12" s="44">
         <v>11</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="42" t="s">
         <v>80</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -3898,19 +3906,19 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A13" s="45">
+      <c r="A13" s="44">
         <v>12</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="43" t="s">
         <v>135</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="42" t="s">
         <v>136</v>
       </c>
       <c r="F13" s="10" t="s">
@@ -3921,19 +3929,19 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A14" s="45">
+      <c r="A14" s="44">
         <v>13</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="43" t="s">
         <v>145</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="42" t="s">
         <v>146</v>
       </c>
       <c r="F14" s="10" t="s">
@@ -3944,19 +3952,19 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A15" s="45">
+      <c r="A15" s="44">
         <v>14</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="43" t="s">
         <v>156</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="42" t="s">
         <v>157</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -3967,16 +3975,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A16" s="45">
+      <c r="A16" s="44">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="6" t="s">
         <v>294</v>
       </c>
@@ -3985,19 +3993,19 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A17" s="45">
+      <c r="A17" s="44">
         <v>16</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="43" t="s">
         <v>84</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="6" t="s">
         <v>294</v>
       </c>
@@ -4006,19 +4014,19 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A18" s="45">
+      <c r="A18" s="44">
         <v>17</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="43" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="42" t="s">
         <v>280</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -4029,19 +4037,19 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A19" s="45">
+      <c r="A19" s="44">
         <v>18</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="43" t="s">
         <v>216</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="42" t="s">
         <v>44</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -4052,16 +4060,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A20" s="45">
+      <c r="A20" s="44">
         <v>19</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="43"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="6" t="s">
         <v>315</v>
       </c>
@@ -4070,16 +4078,16 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A21" s="45">
+      <c r="A21" s="44">
         <v>20</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>405</v>
-      </c>
-      <c r="E21" s="43" t="s">
+      <c r="C21" s="43" t="s">
+        <v>400</v>
+      </c>
+      <c r="E21" s="42" t="s">
         <v>212</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -4090,16 +4098,16 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A22" s="45">
+      <c r="A22" s="44">
         <v>21</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="42" t="s">
         <v>83</v>
       </c>
       <c r="F22" s="6" t="s">
@@ -4110,19 +4118,19 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A23" s="45">
+      <c r="A23" s="44">
         <v>22</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="43" t="s">
         <v>94</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="42" t="s">
         <v>310</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -4133,19 +4141,19 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A24" s="45">
+      <c r="A24" s="44">
         <v>23</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="43" t="s">
         <v>154</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="42" t="s">
         <v>155</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -4156,19 +4164,19 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A25" s="45">
+      <c r="A25" s="44">
         <v>24</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="43" t="s">
         <v>161</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="42" t="s">
         <v>162</v>
       </c>
       <c r="F25" s="10" t="s">
@@ -4179,19 +4187,19 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A26" s="45">
+      <c r="A26" s="44">
         <v>25</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="43" t="s">
         <v>326</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="42" t="s">
         <v>235</v>
       </c>
       <c r="F26" s="10" t="s">
@@ -4202,19 +4210,19 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A27" s="45">
+      <c r="A27" s="44">
         <v>26</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="44" t="s">
-        <v>406</v>
+      <c r="C27" s="43" t="s">
+        <v>401</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="42" t="s">
         <v>276</v>
       </c>
       <c r="F27" s="10" t="s">
@@ -4225,20 +4233,20 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A28" s="45">
+      <c r="A28" s="44">
         <v>27</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="44" t="s">
-        <v>407</v>
+      <c r="C28" s="43" t="s">
+        <v>402</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="43" t="s">
-        <v>408</v>
+      <c r="E28" s="42" t="s">
+        <v>403</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>315</v>
@@ -4248,16 +4256,16 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A29" s="45">
+      <c r="A29" s="44">
         <v>28</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="43" t="s">
         <v>348</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="E29" s="42" t="s">
         <v>347</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -4268,16 +4276,16 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>349</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="E30" s="43" t="s">
+      <c r="E30" s="42" t="s">
         <v>210</v>
       </c>
       <c r="F30" s="6" t="s">
@@ -4288,16 +4296,16 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A31" s="45">
+      <c r="A31" s="44">
         <v>30</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="E31" s="43"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="6" t="s">
         <v>305</v>
       </c>
@@ -4306,19 +4314,19 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A32" s="45">
+      <c r="A32" s="44">
         <v>31</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="44" t="s">
-        <v>409</v>
+      <c r="C32" s="43" t="s">
+        <v>404</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="E32" s="43" t="s">
+      <c r="E32" s="42" t="s">
         <v>307</v>
       </c>
       <c r="F32" s="10" t="s">
@@ -4329,19 +4337,19 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A33" s="45">
+      <c r="A33" s="44">
         <v>32</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="43" t="s">
         <v>89</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="43"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="6" t="s">
         <v>305</v>
       </c>
@@ -4350,19 +4358,19 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A34" s="45">
+      <c r="A34" s="44">
         <v>34</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="43" t="s">
         <v>206</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E34" s="43" t="s">
+      <c r="E34" s="42" t="s">
         <v>344</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -4373,16 +4381,16 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A35" s="45">
+      <c r="A35" s="44">
         <v>35</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="43"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="6" t="s">
         <v>314</v>
       </c>
@@ -4391,19 +4399,19 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A36" s="45">
+      <c r="A36" s="44">
         <v>36</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="43" t="s">
         <v>114</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="42" t="s">
         <v>345</v>
       </c>
       <c r="F36" s="10" t="s">
@@ -4414,19 +4422,19 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A37" s="45">
+      <c r="A37" s="44">
         <v>37</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="44" t="s">
-        <v>410</v>
+      <c r="C37" s="43" t="s">
+        <v>405</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E37" s="43" t="s">
+      <c r="E37" s="42" t="s">
         <v>346</v>
       </c>
       <c r="F37" s="6" t="s">
@@ -4437,19 +4445,19 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A38" s="45">
+      <c r="A38" s="44">
         <v>38</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="43" t="s">
         <v>163</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="42" t="s">
         <v>164</v>
       </c>
       <c r="F38" s="6" t="s">
@@ -4460,19 +4468,19 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A39" s="45">
+      <c r="A39" s="44">
         <v>39</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="44" t="s">
+      <c r="C39" s="43" t="s">
         <v>350</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E39" s="43" t="s">
+      <c r="E39" s="42" t="s">
         <v>171</v>
       </c>
       <c r="F39" s="6" t="s">
@@ -4483,20 +4491,20 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A40" s="45">
+      <c r="A40" s="44">
         <v>40</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="44" t="s">
-        <v>411</v>
+      <c r="C40" s="43" t="s">
+        <v>406</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E40" s="43" t="s">
-        <v>412</v>
+      <c r="E40" s="42" t="s">
+        <v>407</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>5</v>
@@ -4506,19 +4514,19 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A41" s="45">
+      <c r="A41" s="44">
         <v>41</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="44" t="s">
+      <c r="C41" s="43" t="s">
         <v>286</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E41" s="43" t="s">
+      <c r="E41" s="42" t="s">
         <v>43</v>
       </c>
       <c r="F41" s="6" t="s">
@@ -4529,19 +4537,19 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A42" s="45">
+      <c r="A42" s="44">
         <v>42</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="43" t="s">
         <v>141</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="43" t="s">
+      <c r="E42" s="42" t="s">
         <v>142</v>
       </c>
       <c r="F42" s="10" t="s">
@@ -4552,19 +4560,19 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A43" s="45">
+      <c r="A43" s="44">
         <v>43</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="43" t="s">
+      <c r="E43" s="42" t="s">
         <v>200</v>
       </c>
       <c r="F43" s="6" t="s">
@@ -4575,10 +4583,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A44" s="45">
+      <c r="A44" s="44">
         <v>44</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -4587,7 +4595,7 @@
       <c r="D44" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="42" t="s">
         <v>201</v>
       </c>
       <c r="F44" s="6" t="s">
@@ -4598,19 +4606,19 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A45" s="45">
+      <c r="A45" s="44">
         <v>33</v>
       </c>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="43" t="s">
         <v>328</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="42" t="s">
         <v>235</v>
       </c>
       <c r="F45" s="10" t="s">
@@ -4621,19 +4629,19 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A46" s="45">
+      <c r="A46" s="44">
         <v>45</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C46" s="44" t="s">
+      <c r="C46" s="43" t="s">
         <v>158</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E46" s="43" t="s">
+      <c r="E46" s="42" t="s">
         <v>159</v>
       </c>
       <c r="F46" s="6" t="s">
@@ -4644,19 +4652,19 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A47" s="45">
+      <c r="A47" s="44">
         <v>46</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="44" t="s">
-        <v>414</v>
+      <c r="C47" s="43" t="s">
+        <v>409</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E47" s="43" t="s">
+      <c r="E47" s="42" t="s">
         <v>160</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -4667,19 +4675,19 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A48" s="45">
+      <c r="A48" s="44">
         <v>47</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="43" t="s">
         <v>353</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="E48" s="43" t="s">
+      <c r="E48" s="42" t="s">
         <v>50</v>
       </c>
       <c r="F48" s="6" t="s">
@@ -4690,16 +4698,16 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A49" s="45">
+      <c r="A49" s="44">
         <v>48</v>
       </c>
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="44" t="s">
+      <c r="C49" s="43" t="s">
         <v>355</v>
       </c>
-      <c r="E49" s="43" t="s">
+      <c r="E49" s="42" t="s">
         <v>53</v>
       </c>
       <c r="F49" s="6" t="s">
@@ -4710,16 +4718,16 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A50" s="45">
+      <c r="A50" s="44">
         <v>49</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="44" t="s">
+      <c r="C50" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="43" t="s">
+      <c r="E50" s="42" t="s">
         <v>208</v>
       </c>
       <c r="F50" s="6" t="s">
@@ -4730,16 +4738,16 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A51" s="45">
+      <c r="A51" s="44">
         <v>50</v>
       </c>
-      <c r="B51" s="44" t="s">
+      <c r="B51" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="44" t="s">
+      <c r="C51" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="43"/>
+      <c r="E51" s="42"/>
       <c r="F51" s="10" t="s">
         <v>303</v>
       </c>
@@ -4748,19 +4756,19 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A52" s="45">
+      <c r="A52" s="44">
         <v>51</v>
       </c>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="43" t="s">
         <v>95</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E52" s="43" t="s">
+      <c r="E52" s="42" t="s">
         <v>311</v>
       </c>
       <c r="F52" s="10" t="s">
@@ -4771,19 +4779,19 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A53" s="45">
+      <c r="A53" s="44">
         <v>52</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="44" t="s">
+      <c r="C53" s="43" t="s">
         <v>288</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E53" s="43" t="s">
+      <c r="E53" s="42" t="s">
         <v>313</v>
       </c>
       <c r="F53" s="10" t="s">
@@ -4794,19 +4802,19 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A54" s="45">
+      <c r="A54" s="44">
         <v>53</v>
       </c>
-      <c r="B54" s="44" t="s">
+      <c r="B54" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="44" t="s">
+      <c r="C54" s="43" t="s">
         <v>99</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E54" s="43" t="s">
+      <c r="E54" s="42" t="s">
         <v>100</v>
       </c>
       <c r="F54" s="10" t="s">
@@ -4817,19 +4825,19 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A55" s="45">
+      <c r="A55" s="44">
         <v>54</v>
       </c>
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="44" t="s">
+      <c r="C55" s="43" t="s">
         <v>110</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="43" t="s">
+      <c r="E55" s="42" t="s">
         <v>111</v>
       </c>
       <c r="F55" s="10" t="s">
@@ -4840,19 +4848,19 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A56" s="45">
+      <c r="A56" s="44">
         <v>55</v>
       </c>
-      <c r="B56" s="44" t="s">
+      <c r="B56" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="44" t="s">
+      <c r="C56" s="43" t="s">
         <v>254</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="42" t="s">
         <v>255</v>
       </c>
       <c r="F56" s="10" t="s">
@@ -4863,19 +4871,19 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A57" s="45">
+      <c r="A57" s="44">
         <v>56</v>
       </c>
-      <c r="B57" s="44" t="s">
+      <c r="B57" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="44" t="s">
+      <c r="C57" s="43" t="s">
         <v>112</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E57" s="43" t="s">
+      <c r="E57" s="42" t="s">
         <v>113</v>
       </c>
       <c r="F57" s="10" t="s">
@@ -4886,19 +4894,19 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A58" s="45">
+      <c r="A58" s="44">
         <v>57</v>
       </c>
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C58" s="43" t="s">
         <v>120</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E58" s="43" t="s">
+      <c r="E58" s="42" t="s">
         <v>121</v>
       </c>
       <c r="F58" s="10" t="s">
@@ -4909,19 +4917,19 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A59" s="45">
+      <c r="A59" s="44">
         <v>58</v>
       </c>
-      <c r="B59" s="44" t="s">
+      <c r="B59" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C59" s="44" t="s">
+      <c r="C59" s="43" t="s">
         <v>137</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E59" s="43" t="s">
+      <c r="E59" s="42" t="s">
         <v>138</v>
       </c>
       <c r="F59" s="6" t="s">
@@ -4932,19 +4940,19 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A60" s="45">
+      <c r="A60" s="44">
         <v>59</v>
       </c>
-      <c r="B60" s="44" t="s">
+      <c r="B60" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="44" t="s">
+      <c r="C60" s="43" t="s">
         <v>150</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="E60" s="42" t="s">
         <v>151</v>
       </c>
       <c r="F60" s="10" t="s">
@@ -4956,19 +4964,19 @@
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A61" s="45">
+      <c r="A61" s="44">
         <v>60</v>
       </c>
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="44" t="s">
+      <c r="C61" s="43" t="s">
         <v>167</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E61" s="43" t="s">
+      <c r="E61" s="42" t="s">
         <v>168</v>
       </c>
       <c r="F61" s="6" t="s">
@@ -4980,16 +4988,16 @@
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A62" s="45">
+      <c r="A62" s="44">
         <v>61</v>
       </c>
-      <c r="B62" s="44" t="s">
+      <c r="B62" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="43"/>
+      <c r="E62" s="42"/>
       <c r="F62" s="6" t="s">
         <v>301</v>
       </c>
@@ -4999,16 +5007,16 @@
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A63" s="45">
+      <c r="A63" s="44">
         <v>62</v>
       </c>
-      <c r="B63" s="44" t="s">
+      <c r="B63" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C63" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="E63" s="43"/>
+      <c r="C63" s="43" t="s">
+        <v>368</v>
+      </c>
+      <c r="E63" s="42"/>
       <c r="F63" s="10" t="s">
         <v>301</v>
       </c>
@@ -5018,16 +5026,16 @@
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A64" s="45">
+      <c r="A64" s="44">
         <v>63</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="B64" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C64" s="44" t="s">
+      <c r="C64" s="43" t="s">
         <v>318</v>
       </c>
-      <c r="E64" s="43"/>
+      <c r="E64" s="42"/>
       <c r="F64" s="6" t="s">
         <v>301</v>
       </c>
@@ -5037,19 +5045,19 @@
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A65" s="45">
+      <c r="A65" s="44">
         <v>64</v>
       </c>
-      <c r="B65" s="44" t="s">
+      <c r="B65" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="44" t="s">
+      <c r="C65" s="43" t="s">
         <v>87</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E65" s="43"/>
+      <c r="E65" s="42"/>
       <c r="F65" s="6" t="s">
         <v>301</v>
       </c>
@@ -5059,19 +5067,19 @@
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A66" s="45">
+      <c r="A66" s="44">
         <v>65</v>
       </c>
-      <c r="B66" s="44" t="s">
+      <c r="B66" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C66" s="44" t="s">
+      <c r="C66" s="43" t="s">
         <v>287</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="43" t="s">
+      <c r="E66" s="42" t="s">
         <v>107</v>
       </c>
       <c r="F66" s="6" t="s">
@@ -5083,19 +5091,19 @@
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A67" s="45">
+      <c r="A67" s="44">
         <v>66</v>
       </c>
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="43" t="s">
+      <c r="E67" s="42" t="s">
         <v>224</v>
       </c>
       <c r="F67" s="10" t="s">
@@ -5107,19 +5115,19 @@
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A68" s="45">
+      <c r="A68" s="44">
         <v>67</v>
       </c>
-      <c r="B68" s="44" t="s">
+      <c r="B68" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E68" s="43" t="s">
+      <c r="E68" s="42" t="s">
         <v>203</v>
       </c>
       <c r="F68" s="6" t="s">
@@ -5131,19 +5139,19 @@
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A69" s="45">
+      <c r="A69" s="44">
         <v>68</v>
       </c>
-      <c r="B69" s="44" t="s">
+      <c r="B69" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="44" t="s">
+      <c r="C69" s="43" t="s">
         <v>320</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E69" s="43" t="s">
+      <c r="E69" s="42" t="s">
         <v>268</v>
       </c>
       <c r="F69" s="10" t="s">
@@ -5155,19 +5163,19 @@
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A70" s="45">
+      <c r="A70" s="44">
         <v>69</v>
       </c>
-      <c r="B70" s="44" t="s">
+      <c r="B70" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C70" s="44" t="s">
-        <v>372</v>
+      <c r="C70" s="43" t="s">
+        <v>367</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E70" s="43" t="s">
+      <c r="E70" s="42" t="s">
         <v>270</v>
       </c>
       <c r="F70" s="10" t="s">
@@ -5179,19 +5187,19 @@
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A71" s="45">
+      <c r="A71" s="44">
         <v>70</v>
       </c>
-      <c r="B71" s="44" t="s">
+      <c r="B71" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="44" t="s">
+      <c r="C71" s="43" t="s">
         <v>279</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E71" s="43" t="s">
+      <c r="E71" s="42" t="s">
         <v>278</v>
       </c>
       <c r="F71" s="10" t="s">
@@ -5203,19 +5211,19 @@
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A72" s="45">
+      <c r="A72" s="44">
         <v>71</v>
       </c>
-      <c r="B72" s="44" t="s">
+      <c r="B72" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="44" t="s">
-        <v>376</v>
+      <c r="C72" s="43" t="s">
+        <v>371</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E72" s="43" t="s">
+      <c r="E72" s="42" t="s">
         <v>205</v>
       </c>
       <c r="F72" s="6" t="s">
@@ -5227,16 +5235,16 @@
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A73" s="45">
+      <c r="A73" s="44">
         <v>72</v>
       </c>
-      <c r="B73" s="44" t="s">
+      <c r="B73" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C73" s="44" t="s">
+      <c r="C73" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="E73" s="43"/>
+      <c r="E73" s="42"/>
       <c r="F73" s="10" t="s">
         <v>300</v>
       </c>
@@ -5246,16 +5254,16 @@
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A74" s="45">
+      <c r="A74" s="44">
         <v>73</v>
       </c>
-      <c r="B74" s="44" t="s">
+      <c r="B74" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C74" s="44" t="s">
+      <c r="C74" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="43"/>
+      <c r="E74" s="42"/>
       <c r="F74" s="6" t="s">
         <v>300</v>
       </c>
@@ -5265,10 +5273,10 @@
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A75" s="45">
+      <c r="A75" s="44">
         <v>74</v>
       </c>
-      <c r="B75" s="44" t="s">
+      <c r="B75" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C75" s="4" t="s">
@@ -5277,7 +5285,7 @@
       <c r="D75" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E75" s="43" t="s">
+      <c r="E75" s="42" t="s">
         <v>321</v>
       </c>
       <c r="F75" s="6" t="s">
@@ -5289,19 +5297,19 @@
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A76" s="45">
+      <c r="A76" s="44">
         <v>75</v>
       </c>
-      <c r="B76" s="44" t="s">
+      <c r="B76" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E76" s="43" t="s">
+      <c r="E76" s="42" t="s">
         <v>222</v>
       </c>
       <c r="F76" s="10" t="s">
@@ -5313,19 +5321,19 @@
       <c r="H76" s="1"/>
     </row>
     <row r="77" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A77" s="45">
+      <c r="A77" s="44">
         <v>76</v>
       </c>
-      <c r="B77" s="44" t="s">
+      <c r="B77" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E77" s="43" t="s">
+      <c r="E77" s="42" t="s">
         <v>199</v>
       </c>
       <c r="F77" s="6" t="s">
@@ -5337,20 +5345,20 @@
       <c r="H77" s="7"/>
     </row>
     <row r="78" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A78" s="45">
+      <c r="A78" s="44">
         <v>77</v>
       </c>
-      <c r="B78" s="44" t="s">
+      <c r="B78" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E78" s="43" t="s">
-        <v>380</v>
+      <c r="E78" s="42" t="s">
+        <v>375</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>300</v>
@@ -5361,19 +5369,19 @@
       <c r="H78" s="7"/>
     </row>
     <row r="79" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A79" s="45">
+      <c r="A79" s="44">
         <v>78</v>
       </c>
-      <c r="B79" s="44" t="s">
+      <c r="B79" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E79" s="43" t="s">
+      <c r="E79" s="42" t="s">
         <v>324</v>
       </c>
       <c r="F79" s="10" t="s">
@@ -5385,10 +5393,10 @@
       <c r="H79" s="7"/>
     </row>
     <row r="80" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A80" s="45">
+      <c r="A80" s="44">
         <v>79</v>
       </c>
-      <c r="B80" s="44" t="s">
+      <c r="B80" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -5397,7 +5405,7 @@
       <c r="D80" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E80" s="43" t="s">
+      <c r="E80" s="42" t="s">
         <v>231</v>
       </c>
       <c r="F80" s="10" t="s">
@@ -5409,19 +5417,19 @@
       <c r="H80" s="7"/>
     </row>
     <row r="81" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A81" s="45">
+      <c r="A81" s="44">
         <v>80</v>
       </c>
-      <c r="B81" s="44" t="s">
+      <c r="B81" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="44" t="s">
+      <c r="C81" s="43" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E81" s="43" t="s">
+      <c r="E81" s="42" t="s">
         <v>232</v>
       </c>
       <c r="F81" s="10" t="s">
@@ -5433,19 +5441,19 @@
       <c r="H81" s="7"/>
     </row>
     <row r="82" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A82" s="45">
+      <c r="A82" s="44">
         <v>81</v>
       </c>
-      <c r="B82" s="44" t="s">
+      <c r="B82" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C82" s="44" t="s">
+      <c r="C82" s="43" t="s">
         <v>262</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="E82" s="43" t="s">
+      <c r="E82" s="42" t="s">
         <v>266</v>
       </c>
       <c r="F82" s="10" t="s">
@@ -5457,16 +5465,16 @@
       <c r="H82" s="7"/>
     </row>
     <row r="83" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A83" s="45">
+      <c r="A83" s="44">
         <v>82</v>
       </c>
-      <c r="B83" s="44" t="s">
+      <c r="B83" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C83" s="44" t="s">
+      <c r="C83" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="E83" s="43" t="s">
+      <c r="E83" s="42" t="s">
         <v>64</v>
       </c>
       <c r="F83" s="6" t="s">
@@ -5478,16 +5486,16 @@
       <c r="H83" s="7"/>
     </row>
     <row r="84" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A84" s="45">
+      <c r="A84" s="44">
         <v>83</v>
       </c>
-      <c r="B84" s="44" t="s">
+      <c r="B84" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C84" s="44" t="s">
+      <c r="C84" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E84" s="43"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="6" t="s">
         <v>292</v>
       </c>
@@ -5497,20 +5505,20 @@
       <c r="H84" s="7"/>
     </row>
     <row r="85" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A85" s="45">
+      <c r="A85" s="44">
         <v>84</v>
       </c>
-      <c r="B85" s="44" t="s">
+      <c r="B85" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C85" s="44" t="s">
+      <c r="C85" s="43" t="s">
         <v>105</v>
       </c>
       <c r="D85" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E85" s="43" t="s">
-        <v>382</v>
+      <c r="E85" s="42" t="s">
+        <v>377</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>292</v>
@@ -5521,10 +5529,10 @@
       <c r="H85" s="7"/>
     </row>
     <row r="86" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A86" s="45">
+      <c r="A86" s="44">
         <v>85</v>
       </c>
-      <c r="B86" s="44" t="s">
+      <c r="B86" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -5533,7 +5541,7 @@
       <c r="D86" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E86" s="43" t="s">
+      <c r="E86" s="42" t="s">
         <v>221</v>
       </c>
       <c r="F86" s="6" t="s">
@@ -5545,16 +5553,16 @@
       <c r="H86" s="7"/>
     </row>
     <row r="87" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A87" s="45">
+      <c r="A87" s="44">
         <v>86</v>
       </c>
-      <c r="B87" s="44" t="s">
+      <c r="B87" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C87" s="44" t="s">
+      <c r="C87" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E87" s="43"/>
+      <c r="E87" s="42"/>
       <c r="F87" s="6" t="s">
         <v>317</v>
       </c>
@@ -5564,16 +5572,16 @@
       <c r="H87" s="7"/>
     </row>
     <row r="88" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A88" s="45">
+      <c r="A88" s="44">
         <v>87</v>
       </c>
-      <c r="B88" s="44" t="s">
+      <c r="B88" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C88" s="44" t="s">
-        <v>383</v>
-      </c>
-      <c r="E88" s="43" t="s">
+      <c r="C88" s="43" t="s">
+        <v>378</v>
+      </c>
+      <c r="E88" s="42" t="s">
         <v>330</v>
       </c>
       <c r="F88" s="6" t="s">
@@ -5585,19 +5593,19 @@
       <c r="H88" s="7"/>
     </row>
     <row r="89" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A89" s="45">
+      <c r="A89" s="44">
         <v>88</v>
       </c>
-      <c r="B89" s="44" t="s">
+      <c r="B89" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C89" s="44" t="s">
+      <c r="C89" s="43" t="s">
         <v>129</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E89" s="43" t="s">
+      <c r="E89" s="42" t="s">
         <v>130</v>
       </c>
       <c r="F89" s="6" t="s">
@@ -5609,19 +5617,19 @@
       <c r="H89" s="7"/>
     </row>
     <row r="90" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A90" s="45">
+      <c r="A90" s="44">
         <v>89</v>
       </c>
-      <c r="B90" s="44" t="s">
+      <c r="B90" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C90" s="44" t="s">
+      <c r="C90" s="43" t="s">
         <v>152</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E90" s="43" t="s">
+      <c r="E90" s="42" t="s">
         <v>153</v>
       </c>
       <c r="F90" s="6" t="s">
@@ -5633,19 +5641,19 @@
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A91" s="45">
+      <c r="A91" s="44">
         <v>90</v>
       </c>
-      <c r="B91" s="44" t="s">
+      <c r="B91" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C91" s="44" t="s">
+      <c r="C91" s="43" t="s">
         <v>238</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E91" s="43" t="s">
+      <c r="E91" s="42" t="s">
         <v>242</v>
       </c>
       <c r="F91" s="10" t="s">
@@ -5657,17 +5665,17 @@
       <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A92" s="45">
+      <c r="A92" s="44">
         <v>91</v>
       </c>
-      <c r="B92" s="44" t="s">
+      <c r="B92" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C92" s="44" t="s">
+      <c r="C92" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="E92" s="43" t="s">
-        <v>384</v>
+      <c r="E92" s="42" t="s">
+        <v>379</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>302</v>
@@ -5678,16 +5686,16 @@
       <c r="H92" s="8"/>
     </row>
     <row r="93" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A93" s="45">
+      <c r="A93" s="44">
         <v>92</v>
       </c>
-      <c r="B93" s="44" t="s">
+      <c r="B93" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C93" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="E93" s="43" t="s">
+      <c r="C93" s="43" t="s">
+        <v>380</v>
+      </c>
+      <c r="E93" s="42" t="s">
         <v>77</v>
       </c>
       <c r="F93" s="6" t="s">
@@ -5699,10 +5707,10 @@
       <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A94" s="45">
+      <c r="A94" s="44">
         <v>93</v>
       </c>
-      <c r="B94" s="44" t="s">
+      <c r="B94" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -5711,7 +5719,7 @@
       <c r="D94" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E94" s="43" t="s">
+      <c r="E94" s="42" t="s">
         <v>196</v>
       </c>
       <c r="F94" s="6" t="s">
@@ -5723,10 +5731,10 @@
       <c r="H94" s="8"/>
     </row>
     <row r="95" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A95" s="45">
+      <c r="A95" s="44">
         <v>94</v>
       </c>
-      <c r="B95" s="44" t="s">
+      <c r="B95" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -5735,7 +5743,7 @@
       <c r="D95" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="43" t="s">
+      <c r="E95" s="42" t="s">
         <v>197</v>
       </c>
       <c r="F95" s="6" t="s">
@@ -5747,19 +5755,19 @@
       <c r="H95" s="8"/>
     </row>
     <row r="96" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A96" s="45">
+      <c r="A96" s="44">
         <v>95</v>
       </c>
-      <c r="B96" s="44" t="s">
+      <c r="B96" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C96" s="44" t="s">
+      <c r="C96" s="43" t="s">
         <v>173</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E96" s="43" t="s">
+      <c r="E96" s="42" t="s">
         <v>269</v>
       </c>
       <c r="F96" s="10" t="s">
@@ -5771,19 +5779,19 @@
       <c r="H96" s="8"/>
     </row>
     <row r="97" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A97" s="45">
+      <c r="A97" s="44">
         <v>96</v>
       </c>
-      <c r="B97" s="44" t="s">
+      <c r="B97" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C97" s="44" t="s">
+      <c r="C97" s="43" t="s">
         <v>213</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E97" s="43" t="s">
+      <c r="E97" s="42" t="s">
         <v>42</v>
       </c>
       <c r="F97" s="6" t="s">
@@ -5795,16 +5803,16 @@
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A98" s="45">
+      <c r="A98" s="44">
         <v>97</v>
       </c>
-      <c r="B98" s="44" t="s">
+      <c r="B98" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C98" s="44" t="s">
+      <c r="C98" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E98" s="43" t="s">
+      <c r="E98" s="42" t="s">
         <v>284</v>
       </c>
       <c r="F98" s="6" t="s">
@@ -5816,16 +5824,16 @@
       <c r="H98" s="8"/>
     </row>
     <row r="99" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A99" s="45">
+      <c r="A99" s="44">
         <v>98</v>
       </c>
-      <c r="B99" s="44" t="s">
+      <c r="B99" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C99" s="44" t="s">
+      <c r="C99" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="E99" s="43" t="s">
+      <c r="E99" s="42" t="s">
         <v>62</v>
       </c>
       <c r="F99" s="6" t="s">
@@ -5837,19 +5845,19 @@
       <c r="H99" s="8"/>
     </row>
     <row r="100" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A100" s="45">
+      <c r="A100" s="44">
         <v>99</v>
       </c>
-      <c r="B100" s="44" t="s">
+      <c r="B100" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C100" s="44" t="s">
+      <c r="C100" s="43" t="s">
         <v>92</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E100" s="43" t="s">
+      <c r="E100" s="42" t="s">
         <v>309</v>
       </c>
       <c r="F100" s="6" t="s">
@@ -5861,19 +5869,19 @@
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A101" s="45">
+      <c r="A101" s="44">
         <v>100</v>
       </c>
-      <c r="B101" s="44" t="s">
+      <c r="B101" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C101" s="44" t="s">
+      <c r="C101" s="43" t="s">
         <v>131</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E101" s="43" t="s">
+      <c r="E101" s="42" t="s">
         <v>132</v>
       </c>
       <c r="F101" s="6" t="s">
@@ -5885,19 +5893,19 @@
       <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A102" s="45">
+      <c r="A102" s="44">
         <v>101</v>
       </c>
-      <c r="B102" s="44" t="s">
+      <c r="B102" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C102" s="44" t="s">
+      <c r="C102" s="43" t="s">
         <v>147</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E102" s="43" t="s">
+      <c r="E102" s="42" t="s">
         <v>148</v>
       </c>
       <c r="F102" s="6" t="s">
@@ -5909,19 +5917,19 @@
       <c r="H102" s="8"/>
     </row>
     <row r="103" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A103" s="45">
+      <c r="A103" s="44">
         <v>102</v>
       </c>
-      <c r="B103" s="44" t="s">
+      <c r="B103" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C103" s="44" t="s">
+      <c r="C103" s="43" t="s">
         <v>149</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E103" s="43" t="s">
+      <c r="E103" s="42" t="s">
         <v>259</v>
       </c>
       <c r="F103" s="6" t="s">
@@ -5932,19 +5940,19 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A104" s="45">
+      <c r="A104" s="44">
         <v>103</v>
       </c>
-      <c r="B104" s="44" t="s">
+      <c r="B104" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E104" s="43" t="s">
+      <c r="E104" s="42" t="s">
         <v>223</v>
       </c>
       <c r="F104" s="6" t="s">
@@ -5956,10 +5964,10 @@
       <c r="H104" s="8"/>
     </row>
     <row r="105" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A105" s="45">
+      <c r="A105" s="44">
         <v>104</v>
       </c>
-      <c r="B105" s="44" t="s">
+      <c r="B105" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C105" s="4" t="s">
@@ -5968,7 +5976,7 @@
       <c r="D105" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E105" s="43" t="s">
+      <c r="E105" s="42" t="s">
         <v>202</v>
       </c>
       <c r="F105" s="6" t="s">
@@ -5980,10 +5988,10 @@
       <c r="H105" s="8"/>
     </row>
     <row r="106" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A106" s="45">
+      <c r="A106" s="44">
         <v>105</v>
       </c>
-      <c r="B106" s="44" t="s">
+      <c r="B106" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C106" s="4" t="s">
@@ -5992,7 +6000,7 @@
       <c r="D106" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E106" s="43" t="s">
+      <c r="E106" s="42" t="s">
         <v>323</v>
       </c>
       <c r="F106" s="10" t="s">
@@ -6004,19 +6012,19 @@
       <c r="H106" s="8"/>
     </row>
     <row r="107" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A107" s="45">
+      <c r="A107" s="44">
         <v>106</v>
       </c>
-      <c r="B107" s="44" t="s">
+      <c r="B107" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C107" s="44" t="s">
+      <c r="C107" s="43" t="s">
         <v>263</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="E107" s="43" t="s">
+      <c r="E107" s="42" t="s">
         <v>261</v>
       </c>
       <c r="F107" s="10" t="s">
@@ -6028,19 +6036,19 @@
       <c r="H107" s="8"/>
     </row>
     <row r="108" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A108" s="45">
+      <c r="A108" s="44">
         <v>107</v>
       </c>
-      <c r="B108" s="44" t="s">
+      <c r="B108" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C108" s="44" t="s">
+      <c r="C108" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E108" s="43" t="s">
+      <c r="E108" s="42" t="s">
         <v>267</v>
       </c>
       <c r="F108" s="10" t="s">
@@ -6052,16 +6060,16 @@
       <c r="H108" s="8"/>
     </row>
     <row r="109" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A109" s="45">
+      <c r="A109" s="44">
         <v>108</v>
       </c>
-      <c r="B109" s="44" t="s">
+      <c r="B109" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C109" s="44" t="s">
-        <v>387</v>
-      </c>
-      <c r="E109" s="43" t="s">
+      <c r="C109" s="43" t="s">
+        <v>382</v>
+      </c>
+      <c r="E109" s="42" t="s">
         <v>297</v>
       </c>
       <c r="F109" s="10" t="s">
@@ -6073,16 +6081,16 @@
       <c r="H109" s="8"/>
     </row>
     <row r="110" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A110" s="45">
+      <c r="A110" s="44">
         <v>109</v>
       </c>
-      <c r="B110" s="44" t="s">
+      <c r="B110" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C110" s="44" t="s">
+      <c r="C110" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="E110" s="43"/>
+      <c r="E110" s="42"/>
       <c r="F110" s="10" t="s">
         <v>298</v>
       </c>
@@ -6092,19 +6100,19 @@
       <c r="H110" s="8"/>
     </row>
     <row r="111" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A111" s="45">
+      <c r="A111" s="44">
         <v>110</v>
       </c>
-      <c r="B111" s="44" t="s">
+      <c r="B111" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C111" s="44" t="s">
+      <c r="C111" s="43" t="s">
         <v>287</v>
       </c>
       <c r="D111" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E111" s="43" t="s">
+      <c r="E111" s="42" t="s">
         <v>106</v>
       </c>
       <c r="F111" s="6" t="s">
@@ -6116,19 +6124,19 @@
       <c r="H111" s="8"/>
     </row>
     <row r="112" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A112" s="45">
+      <c r="A112" s="44">
         <v>111</v>
       </c>
-      <c r="B112" s="44" t="s">
+      <c r="B112" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C112" s="44" t="s">
+      <c r="C112" s="43" t="s">
         <v>165</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E112" s="43" t="s">
+      <c r="E112" s="42" t="s">
         <v>166</v>
       </c>
       <c r="F112" s="6" t="s">
@@ -6140,17 +6148,17 @@
       <c r="H112" s="9"/>
     </row>
     <row r="113" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A113" s="45">
+      <c r="A113" s="44">
         <v>112</v>
       </c>
-      <c r="B113" s="44" t="s">
+      <c r="B113" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C113" s="44" t="s">
+      <c r="C113" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E113" s="43" t="s">
-        <v>388</v>
+      <c r="E113" s="42" t="s">
+        <v>383</v>
       </c>
       <c r="F113" s="10" t="s">
         <v>291</v>
@@ -6161,19 +6169,19 @@
       <c r="H113" s="9"/>
     </row>
     <row r="114" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A114" s="45">
+      <c r="A114" s="44">
         <v>113</v>
       </c>
-      <c r="B114" s="44" t="s">
+      <c r="B114" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C114" s="44" t="s">
+      <c r="C114" s="43" t="s">
         <v>126</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E114" s="43" t="s">
+      <c r="E114" s="42" t="s">
         <v>127</v>
       </c>
       <c r="F114" s="10" t="s">
@@ -6184,19 +6192,19 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A115" s="45">
+      <c r="A115" s="44">
         <v>114</v>
       </c>
-      <c r="B115" s="44" t="s">
+      <c r="B115" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C115" s="44" t="s">
+      <c r="C115" s="43" t="s">
         <v>169</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E115" s="43" t="s">
+      <c r="E115" s="42" t="s">
         <v>170</v>
       </c>
       <c r="F115" s="6" t="s">
@@ -6207,19 +6215,19 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A116" s="45">
+      <c r="A116" s="44">
         <v>115</v>
       </c>
-      <c r="B116" s="44" t="s">
+      <c r="B116" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C116" s="44" t="s">
-        <v>389</v>
+      <c r="C116" s="43" t="s">
+        <v>384</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="E116" s="43" t="s">
+      <c r="E116" s="42" t="s">
         <v>45</v>
       </c>
       <c r="F116" s="6" t="s">
@@ -6230,16 +6238,16 @@
       </c>
     </row>
     <row r="117" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A117" s="45">
+      <c r="A117" s="44">
         <v>116</v>
       </c>
-      <c r="B117" s="44" t="s">
+      <c r="B117" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C117" s="44" t="s">
+      <c r="C117" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E117" s="43" t="s">
+      <c r="E117" s="42" t="s">
         <v>209</v>
       </c>
       <c r="F117" s="6" t="s">
@@ -6250,16 +6258,16 @@
       </c>
     </row>
     <row r="118" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A118" s="45">
+      <c r="A118" s="44">
         <v>117</v>
       </c>
-      <c r="B118" s="44" t="s">
+      <c r="B118" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C118" s="44" t="s">
+      <c r="C118" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E118" s="43"/>
+      <c r="E118" s="42"/>
       <c r="F118" s="6" t="s">
         <v>204</v>
       </c>
@@ -6268,16 +6276,16 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A119" s="45">
+      <c r="A119" s="44">
         <v>118</v>
       </c>
-      <c r="B119" s="44" t="s">
+      <c r="B119" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C119" s="44" t="s">
+      <c r="C119" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E119" s="43" t="s">
+      <c r="E119" s="42" t="s">
         <v>69</v>
       </c>
       <c r="F119" s="6" t="s">
@@ -6288,16 +6296,16 @@
       </c>
     </row>
     <row r="120" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A120" s="45">
+      <c r="A120" s="44">
         <v>119</v>
       </c>
-      <c r="B120" s="44" t="s">
+      <c r="B120" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C120" s="44" t="s">
-        <v>390</v>
-      </c>
-      <c r="E120" s="43" t="s">
+      <c r="C120" s="43" t="s">
+        <v>385</v>
+      </c>
+      <c r="E120" s="42" t="s">
         <v>72</v>
       </c>
       <c r="F120" s="6" t="s">
@@ -6308,19 +6316,19 @@
       </c>
     </row>
     <row r="121" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A121" s="45">
+      <c r="A121" s="44">
         <v>120</v>
       </c>
-      <c r="B121" s="44" t="s">
+      <c r="B121" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C121" s="44" t="s">
+      <c r="C121" s="43" t="s">
         <v>237</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="E121" s="43" t="s">
+      <c r="E121" s="42" t="s">
         <v>243</v>
       </c>
       <c r="F121" s="10" t="s">
@@ -6331,19 +6339,19 @@
       </c>
     </row>
     <row r="122" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A122" s="45">
+      <c r="A122" s="44">
         <v>121</v>
       </c>
-      <c r="B122" s="44" t="s">
+      <c r="B122" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C122" s="44" t="s">
+      <c r="C122" s="43" t="s">
         <v>139</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E122" s="43" t="s">
+      <c r="E122" s="42" t="s">
         <v>140</v>
       </c>
       <c r="F122" s="10" t="s">
@@ -6354,19 +6362,19 @@
       </c>
     </row>
     <row r="123" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A123" s="45">
+      <c r="A123" s="44">
         <v>122</v>
       </c>
-      <c r="B123" s="44" t="s">
+      <c r="B123" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C123" s="44" t="s">
+      <c r="C123" s="43" t="s">
         <v>143</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E123" s="43" t="s">
+      <c r="E123" s="42" t="s">
         <v>144</v>
       </c>
       <c r="F123" s="6" t="s">
@@ -6377,16 +6385,16 @@
       </c>
     </row>
     <row r="124" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A124" s="45">
+      <c r="A124" s="44">
         <v>123</v>
       </c>
-      <c r="B124" s="44" t="s">
+      <c r="B124" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C124" s="44" t="s">
+      <c r="C124" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E124" s="43"/>
+      <c r="E124" s="42"/>
       <c r="F124" s="6" t="s">
         <v>295</v>
       </c>
@@ -6395,19 +6403,19 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A125" s="45">
+      <c r="A125" s="44">
         <v>124</v>
       </c>
-      <c r="B125" s="44" t="s">
+      <c r="B125" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C125" s="44" t="s">
+      <c r="C125" s="43" t="s">
         <v>93</v>
       </c>
       <c r="D125" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E125" s="43" t="s">
+      <c r="E125" s="42" t="s">
         <v>308</v>
       </c>
       <c r="F125" s="10" t="s">
@@ -6418,20 +6426,20 @@
       </c>
     </row>
     <row r="126" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A126" s="45">
+      <c r="A126" s="44">
         <v>125</v>
       </c>
-      <c r="B126" s="44" t="s">
+      <c r="B126" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C126" s="44" t="s">
+      <c r="C126" s="43" t="s">
         <v>96</v>
       </c>
       <c r="D126" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E126" s="43" t="s">
-        <v>391</v>
+      <c r="E126" s="42" t="s">
+        <v>386</v>
       </c>
       <c r="F126" s="10" t="s">
         <v>295</v>
@@ -6441,19 +6449,19 @@
       </c>
     </row>
     <row r="127" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A127" s="45">
+      <c r="A127" s="44">
         <v>126</v>
       </c>
-      <c r="B127" s="44" t="s">
+      <c r="B127" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C127" s="44" t="s">
+      <c r="C127" s="43" t="s">
         <v>97</v>
       </c>
       <c r="D127" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E127" s="43" t="s">
+      <c r="E127" s="42" t="s">
         <v>98</v>
       </c>
       <c r="F127" s="10" t="s">
@@ -6464,19 +6472,19 @@
       </c>
     </row>
     <row r="128" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A128" s="45">
+      <c r="A128" s="44">
         <v>127</v>
       </c>
-      <c r="B128" s="44" t="s">
+      <c r="B128" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C128" s="44" t="s">
+      <c r="C128" s="43" t="s">
         <v>103</v>
       </c>
       <c r="D128" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E128" s="43" t="s">
+      <c r="E128" s="42" t="s">
         <v>104</v>
       </c>
       <c r="F128" s="10" t="s">
@@ -6487,19 +6495,19 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A129" s="45">
+      <c r="A129" s="44">
         <v>128</v>
       </c>
-      <c r="B129" s="44" t="s">
+      <c r="B129" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C129" s="44" t="s">
+      <c r="C129" s="43" t="s">
         <v>108</v>
       </c>
       <c r="D129" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E129" s="43" t="s">
+      <c r="E129" s="42" t="s">
         <v>109</v>
       </c>
       <c r="F129" s="10" t="s">
@@ -6510,19 +6518,19 @@
       </c>
     </row>
     <row r="130" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A130" s="45">
+      <c r="A130" s="44">
         <v>129</v>
       </c>
-      <c r="B130" s="44" t="s">
+      <c r="B130" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="44" t="s">
+      <c r="C130" s="43" t="s">
         <v>122</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E130" s="43" t="s">
+      <c r="E130" s="42" t="s">
         <v>123</v>
       </c>
       <c r="F130" s="10" t="s">
@@ -6533,19 +6541,19 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A131" s="45">
+      <c r="A131" s="44">
         <v>130</v>
       </c>
-      <c r="B131" s="44" t="s">
+      <c r="B131" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C131" s="44" t="s">
+      <c r="C131" s="43" t="s">
         <v>124</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E131" s="43" t="s">
+      <c r="E131" s="42" t="s">
         <v>125</v>
       </c>
       <c r="F131" s="10" t="s">
@@ -6556,19 +6564,19 @@
       </c>
     </row>
     <row r="132" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A132" s="45">
+      <c r="A132" s="44">
         <v>131</v>
       </c>
-      <c r="B132" s="44" t="s">
+      <c r="B132" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C132" s="44" t="s">
+      <c r="C132" s="43" t="s">
         <v>133</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E132" s="43" t="s">
+      <c r="E132" s="42" t="s">
         <v>134</v>
       </c>
       <c r="F132" s="10" t="s">
@@ -6579,10 +6587,10 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A133" s="45">
+      <c r="A133" s="44">
         <v>132</v>
       </c>
-      <c r="B133" s="44" t="s">
+      <c r="B133" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="4" t="s">
@@ -6591,7 +6599,7 @@
       <c r="D133" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="E133" s="43" t="s">
+      <c r="E133" s="42" t="s">
         <v>229</v>
       </c>
       <c r="F133" s="10" t="s">
@@ -6602,19 +6610,19 @@
       </c>
     </row>
     <row r="134" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A134" s="45">
+      <c r="A134" s="44">
         <v>133</v>
       </c>
-      <c r="B134" s="44" t="s">
+      <c r="B134" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C134" s="44" t="s">
+      <c r="C134" s="43" t="s">
         <v>271</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="E134" s="43" t="s">
+      <c r="E134" s="42" t="s">
         <v>275</v>
       </c>
       <c r="F134" s="10" t="s">
@@ -6625,16 +6633,16 @@
       </c>
     </row>
     <row r="135" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A135" s="45">
+      <c r="A135" s="44">
         <v>134</v>
       </c>
-      <c r="B135" s="44" t="s">
+      <c r="B135" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C135" s="44" t="s">
+      <c r="C135" s="43" t="s">
         <v>281</v>
       </c>
-      <c r="E135" s="43" t="s">
+      <c r="E135" s="42" t="s">
         <v>48</v>
       </c>
       <c r="F135" s="6" t="s">
@@ -6645,16 +6653,16 @@
       </c>
     </row>
     <row r="136" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A136" s="45">
+      <c r="A136" s="44">
         <v>135</v>
       </c>
-      <c r="B136" s="44" t="s">
+      <c r="B136" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C136" s="44" t="s">
+      <c r="C136" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E136" s="43" t="s">
+      <c r="E136" s="42" t="s">
         <v>285</v>
       </c>
       <c r="F136" s="6" t="s">
@@ -6665,17 +6673,17 @@
       </c>
     </row>
     <row r="137" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A137" s="45">
+      <c r="A137" s="44">
         <v>136</v>
       </c>
-      <c r="B137" s="44" t="s">
+      <c r="B137" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C137" s="44" t="s">
+      <c r="C137" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="E137" s="43" t="s">
-        <v>392</v>
+      <c r="E137" s="42" t="s">
+        <v>387</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>304</v>
@@ -6685,16 +6693,16 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A138" s="45">
+      <c r="A138" s="44">
         <v>137</v>
       </c>
-      <c r="B138" s="44" t="s">
+      <c r="B138" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C138" s="44" t="s">
+      <c r="C138" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="E138" s="43"/>
+      <c r="E138" s="42"/>
       <c r="F138" s="6" t="s">
         <v>304</v>
       </c>
@@ -6703,19 +6711,19 @@
       </c>
     </row>
     <row r="139" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A139" s="45">
+      <c r="A139" s="44">
         <v>138</v>
       </c>
-      <c r="B139" s="44" t="s">
+      <c r="B139" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C139" s="44" t="s">
+      <c r="C139" s="43" t="s">
         <v>251</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E139" s="43"/>
+      <c r="E139" s="42"/>
       <c r="F139" s="6" t="s">
         <v>304</v>
       </c>
@@ -6724,19 +6732,19 @@
       </c>
     </row>
     <row r="140" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A140" s="45">
+      <c r="A140" s="44">
         <v>139</v>
       </c>
-      <c r="B140" s="44" t="s">
+      <c r="B140" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C140" s="44" t="s">
-        <v>393</v>
+      <c r="C140" s="43" t="s">
+        <v>388</v>
       </c>
       <c r="D140" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E140" s="43" t="s">
+      <c r="E140" s="42" t="s">
         <v>312</v>
       </c>
       <c r="F140" s="6" t="s">
@@ -6747,19 +6755,19 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A141" s="45">
+      <c r="A141" s="44">
         <v>140</v>
       </c>
-      <c r="B141" s="44" t="s">
+      <c r="B141" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C141" s="44" t="s">
+      <c r="C141" s="43" t="s">
         <v>101</v>
       </c>
       <c r="D141" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E141" s="43" t="s">
+      <c r="E141" s="42" t="s">
         <v>102</v>
       </c>
       <c r="F141" s="10" t="s">
@@ -6770,20 +6778,20 @@
       </c>
     </row>
     <row r="142" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A142" s="45">
+      <c r="A142" s="44">
         <v>141</v>
       </c>
-      <c r="B142" s="44" t="s">
+      <c r="B142" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C142" s="44" t="s">
+      <c r="C142" s="43" t="s">
         <v>252</v>
       </c>
       <c r="D142" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E142" s="43" t="s">
-        <v>394</v>
+      <c r="E142" s="42" t="s">
+        <v>389</v>
       </c>
       <c r="F142" s="10" t="s">
         <v>304</v>
@@ -6793,19 +6801,19 @@
       </c>
     </row>
     <row r="143" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A143" s="45">
+      <c r="A143" s="44">
         <v>142</v>
       </c>
-      <c r="B143" s="44" t="s">
+      <c r="B143" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C143" s="44" t="s">
-        <v>395</v>
+      <c r="C143" s="43" t="s">
+        <v>390</v>
       </c>
       <c r="D143" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E143" s="43" t="s">
+      <c r="E143" s="42" t="s">
         <v>253</v>
       </c>
       <c r="F143" s="10" t="s">
@@ -6816,19 +6824,19 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A144" s="45">
+      <c r="A144" s="44">
         <v>143</v>
       </c>
-      <c r="B144" s="44" t="s">
+      <c r="B144" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C144" s="44" t="s">
+      <c r="C144" s="43" t="s">
         <v>115</v>
       </c>
       <c r="D144" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E144" s="43" t="s">
+      <c r="E144" s="42" t="s">
         <v>116</v>
       </c>
       <c r="F144" s="6" t="s">
@@ -6839,19 +6847,19 @@
       </c>
     </row>
     <row r="145" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A145" s="45">
+      <c r="A145" s="44">
         <v>144</v>
       </c>
-      <c r="B145" s="44" t="s">
+      <c r="B145" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C145" s="44" t="s">
+      <c r="C145" s="43" t="s">
         <v>256</v>
       </c>
       <c r="D145" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E145" s="43" t="s">
+      <c r="E145" s="42" t="s">
         <v>117</v>
       </c>
       <c r="F145" s="6" t="s">
@@ -6862,19 +6870,19 @@
       </c>
     </row>
     <row r="146" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A146" s="45">
+      <c r="A146" s="44">
         <v>145</v>
       </c>
-      <c r="B146" s="44" t="s">
+      <c r="B146" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C146" s="44" t="s">
+      <c r="C146" s="43" t="s">
         <v>257</v>
       </c>
       <c r="D146" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E146" s="43" t="s">
+      <c r="E146" s="42" t="s">
         <v>118</v>
       </c>
       <c r="F146" s="6" t="s">
@@ -6885,19 +6893,19 @@
       </c>
     </row>
     <row r="147" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A147" s="45">
+      <c r="A147" s="44">
         <v>146</v>
       </c>
-      <c r="B147" s="44" t="s">
+      <c r="B147" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C147" s="44" t="s">
+      <c r="C147" s="43" t="s">
         <v>258</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E147" s="43" t="s">
+      <c r="E147" s="42" t="s">
         <v>119</v>
       </c>
       <c r="F147" s="6" t="s">
@@ -6908,10 +6916,10 @@
       </c>
     </row>
     <row r="148" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A148" s="45">
+      <c r="A148" s="44">
         <v>147</v>
       </c>
-      <c r="B148" s="44" t="s">
+      <c r="B148" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C148" s="4" t="s">
@@ -6920,7 +6928,7 @@
       <c r="D148" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E148" s="43" t="s">
+      <c r="E148" s="42" t="s">
         <v>230</v>
       </c>
       <c r="F148" s="10" t="s">
@@ -6931,20 +6939,20 @@
       </c>
     </row>
     <row r="149" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A149" s="45">
+      <c r="A149" s="44">
         <v>148</v>
       </c>
-      <c r="B149" s="44" t="s">
+      <c r="B149" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E149" s="43" t="s">
-        <v>397</v>
+      <c r="E149" s="42" t="s">
+        <v>392</v>
       </c>
       <c r="F149" s="10" t="s">
         <v>299</v>
@@ -6954,19 +6962,19 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A150" s="45">
+      <c r="A150" s="44">
         <v>149</v>
       </c>
-      <c r="B150" s="44" t="s">
+      <c r="B150" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C150" s="44" t="s">
+      <c r="C150" s="43" t="s">
         <v>236</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E150" s="43" t="s">
+      <c r="E150" s="42" t="s">
         <v>241</v>
       </c>
       <c r="F150" s="10" t="s">
@@ -6977,19 +6985,19 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="50.1" customHeight="1">
-      <c r="A151" s="45">
+      <c r="A151" s="44">
         <v>150</v>
       </c>
-      <c r="B151" s="44" t="s">
+      <c r="B151" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C151" s="44" t="s">
+      <c r="C151" s="43" t="s">
         <v>176</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="E151" s="43" t="s">
+      <c r="E151" s="42" t="s">
         <v>277</v>
       </c>
       <c r="F151" s="10" t="s">
@@ -7832,8 +7840,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7902,7 +7910,7 @@
         <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
@@ -8006,29 +8014,23 @@
       <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:37" ht="15.75" thickBot="1">
-      <c r="C14" s="35"/>
-      <c r="D14" s="28" t="s">
+      <c r="C14" s="35" t="s">
         <v>338</v>
       </c>
+      <c r="D14" s="28"/>
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="28" t="s">
-        <v>338</v>
-      </c>
+      <c r="F14" s="28"/>
       <c r="G14" s="41">
         <v>0</v>
       </c>
-      <c r="H14" s="28" t="s">
-        <v>338</v>
-      </c>
+      <c r="H14" s="28"/>
       <c r="I14" s="41">
         <v>0</v>
       </c>
-      <c r="J14" s="28" t="s">
-        <v>338</v>
-      </c>
-      <c r="K14" s="42">
+      <c r="J14" s="28"/>
+      <c r="K14" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8085,11 +8087,11 @@
         <v>332</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25" t="s">
@@ -8103,7 +8105,7 @@
     </row>
     <row r="18" spans="3:13">
       <c r="C18" s="34" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="25">
@@ -8124,22 +8126,22 @@
     </row>
     <row r="19" spans="3:13" ht="15.75" thickBot="1">
       <c r="C19" s="35" t="s">
-        <v>365</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46">
+        <v>360</v>
+      </c>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45">
         <v>0</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46">
+      <c r="F19" s="45"/>
+      <c r="G19" s="45">
         <v>0</v>
       </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46">
+      <c r="H19" s="45"/>
+      <c r="I19" s="45">
         <v>0</v>
       </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="47">
+      <c r="J19" s="45"/>
+      <c r="K19" s="46">
         <v>0</v>
       </c>
     </row>
@@ -8185,96 +8187,120 @@
       </c>
       <c r="M21" s="31"/>
     </row>
-    <row r="22" spans="3:13" ht="15.75" thickBot="1">
-      <c r="C22" s="35" t="s">
-        <v>332</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>356</v>
-      </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28" t="s">
-        <v>359</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28" t="s">
-        <v>357</v>
-      </c>
-      <c r="M22" s="29"/>
+    <row r="22" spans="3:13">
+      <c r="C22" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>411</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27" t="s">
+        <v>415</v>
+      </c>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="M22" s="49"/>
     </row>
     <row r="23" spans="3:13">
-      <c r="C23" s="34"/>
-      <c r="D23" s="48" t="s">
-        <v>371</v>
-      </c>
-      <c r="E23" s="27">
+      <c r="C23" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="25">
         <v>0</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25">
+        <v>0</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25">
+        <v>0</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25">
+        <v>0</v>
+      </c>
+      <c r="L23" s="25"/>
+      <c r="M23" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="3:13">
-      <c r="C24" s="34"/>
-      <c r="D24" s="48" t="s">
-        <v>369</v>
-      </c>
-      <c r="E24" s="27">
+      <c r="C24" s="50" t="s">
+        <v>364</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="25">
         <v>0</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25">
+        <v>0</v>
+      </c>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25">
+        <v>0</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25">
+        <v>0</v>
+      </c>
+      <c r="L24" s="25"/>
+      <c r="M24" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="3:13" ht="15.75" thickBot="1">
-      <c r="C25" s="34"/>
-      <c r="D25" s="48" t="s">
-        <v>370</v>
-      </c>
-      <c r="E25" s="27">
+      <c r="C25" s="51" t="s">
+        <v>365</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="45">
         <v>0</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45">
+        <v>0</v>
+      </c>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45">
+        <v>0</v>
+      </c>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45">
+        <v>0</v>
+      </c>
+      <c r="L25" s="45"/>
+      <c r="M25" s="46">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="3:13">
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="47" t="s">
         <v>333</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
     </row>
     <row r="27" spans="3:13">
       <c r="C27" s="33" t="s">
@@ -8298,15 +8324,15 @@
         <v>332</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="28" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I28" s="29"/>
     </row>

</xml_diff>

<commit_message>
Data analysis report secton done
</commit_message>
<xml_diff>
--- a/Thematic-Coding-Analysis-Tool.xlsx
+++ b/Thematic-Coding-Analysis-Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\Dropbox\Kieran Third year\BCIS301 _ AMIC700\Assignment 1\BCIS301---AMIC700---Thematic-Coding-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4201815D-42E4-4288-AE2F-C0CF809E790B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A49A5D-7722-4EC5-9990-1324379B0A2C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantitative" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="420">
   <si>
     <t>Extract</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,10 +210,6 @@
   </si>
   <si>
     <t>all occurring in parallel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>During the service design and development phase, the intended pilot and phased rollout of the service were removed from the project plan   P7,6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1464,6 +1460,12 @@
   </si>
   <si>
     <t>The project did not take into account the expectations of the target audience at the beginning. Lead to failure to meet specific requirements.</t>
+  </si>
+  <si>
+    <t>During the service design and development phase, the intended pilot and phased rollout of the service were removed from the project plan</t>
+  </si>
+  <si>
+    <t>P7,6</t>
   </si>
 </sst>
 </file>
@@ -3649,8 +3651,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView topLeftCell="A16" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3669,10 +3671,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="26.45" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -3687,7 +3689,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="50.1" customHeight="1">
@@ -3698,16 +3700,16 @@
         <v>41</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="50.1" customHeight="1">
@@ -3718,14 +3720,14 @@
         <v>41</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="50.1" customHeight="1">
@@ -3736,14 +3738,14 @@
         <v>41</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="50.1" customHeight="1">
@@ -3754,16 +3756,16 @@
         <v>41</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="50.1" customHeight="1">
@@ -3774,19 +3776,19 @@
         <v>41</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="50.1" customHeight="1">
@@ -3797,19 +3799,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="50.1" customHeight="1">
@@ -3826,13 +3828,13 @@
         <v>32</v>
       </c>
       <c r="E8" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>227</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="50.1" customHeight="1">
@@ -3843,16 +3845,19 @@
         <v>41</v>
       </c>
       <c r="C9" s="28" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>46</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="50.1" customHeight="1">
@@ -3863,16 +3868,16 @@
         <v>41</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="50.1" customHeight="1">
@@ -3883,16 +3888,16 @@
         <v>41</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.1" customHeight="1">
@@ -3903,16 +3908,16 @@
         <v>41</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>74</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="50.1" customHeight="1">
@@ -3920,22 +3925,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>123</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="50.1" customHeight="1">
@@ -3943,22 +3948,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>132</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="50.1" customHeight="1">
@@ -3966,22 +3971,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>140</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="50.1" customHeight="1">
@@ -3992,14 +3997,14 @@
         <v>41</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="50.1" customHeight="1">
@@ -4010,17 +4015,17 @@
         <v>41</v>
       </c>
       <c r="C17" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="50.1" customHeight="1">
@@ -4037,13 +4042,13 @@
         <v>38</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="50.1" customHeight="1">
@@ -4054,19 +4059,19 @@
         <v>41</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>43</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="50.1" customHeight="1">
@@ -4077,14 +4082,14 @@
         <v>41</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="50.1" customHeight="1">
@@ -4095,16 +4100,16 @@
         <v>41</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="50.1" customHeight="1">
@@ -4115,16 +4120,16 @@
         <v>41</v>
       </c>
       <c r="C22" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="27" t="s">
-        <v>77</v>
-      </c>
       <c r="F22" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="50.1" customHeight="1">
@@ -4132,22 +4137,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="50.1" customHeight="1">
@@ -4155,22 +4160,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>138</v>
-      </c>
       <c r="F24" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="50.1" customHeight="1">
@@ -4178,22 +4183,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>145</v>
-      </c>
       <c r="F25" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="50.1" customHeight="1">
@@ -4204,19 +4209,19 @@
         <v>7</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E26" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="E26" s="27" t="s">
-        <v>218</v>
-      </c>
       <c r="F26" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="50.1" customHeight="1">
@@ -4227,19 +4232,19 @@
         <v>7</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="50.1" customHeight="1">
@@ -4250,19 +4255,19 @@
         <v>7</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="50.1" customHeight="1">
@@ -4273,36 +4278,36 @@
         <v>41</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="50.1" customHeight="1">
       <c r="A30" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="50.1" customHeight="1">
@@ -4313,14 +4318,14 @@
         <v>41</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="50.1" customHeight="1">
@@ -4331,19 +4336,19 @@
         <v>41</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E32" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="E32" s="27" t="s">
-        <v>290</v>
-      </c>
       <c r="F32" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="50.1" customHeight="1">
@@ -4354,17 +4359,17 @@
         <v>41</v>
       </c>
       <c r="C33" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="50.1" customHeight="1">
@@ -4375,19 +4380,19 @@
         <v>41</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="50.1" customHeight="1">
@@ -4398,14 +4403,14 @@
         <v>41</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="50.1" customHeight="1">
@@ -4413,22 +4418,22 @@
         <v>36</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="50.1" customHeight="1">
@@ -4436,22 +4441,22 @@
         <v>37</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="50.1" customHeight="1">
@@ -4459,22 +4464,22 @@
         <v>38</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E38" s="27" t="s">
-        <v>147</v>
-      </c>
       <c r="F38" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="50.1" customHeight="1">
@@ -4482,22 +4487,22 @@
         <v>39</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="50.1" customHeight="1">
@@ -4508,19 +4513,19 @@
         <v>41</v>
       </c>
       <c r="C40" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="27" t="s">
         <v>387</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E40" s="27" t="s">
-        <v>388</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="50.1" customHeight="1">
@@ -4531,10 +4536,10 @@
         <v>41</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E41" s="27" t="s">
         <v>42</v>
@@ -4543,7 +4548,7 @@
         <v>5</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="50.1" customHeight="1">
@@ -4551,22 +4556,22 @@
         <v>42</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C42" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>128</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="50.1" customHeight="1">
@@ -4577,19 +4582,19 @@
         <v>7</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="50.1" customHeight="1">
@@ -4600,19 +4605,19 @@
         <v>7</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="50.1" customHeight="1">
@@ -4623,19 +4628,19 @@
         <v>7</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="50.1" customHeight="1">
@@ -4643,22 +4648,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>142</v>
-      </c>
       <c r="F46" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="50.1" customHeight="1">
@@ -4666,22 +4671,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="50.1" customHeight="1">
@@ -4692,19 +4697,19 @@
         <v>41</v>
       </c>
       <c r="C48" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>337</v>
-      </c>
       <c r="E48" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="50.1" customHeight="1">
@@ -4715,16 +4720,16 @@
         <v>41</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="50.1" customHeight="1">
@@ -4735,16 +4740,16 @@
         <v>41</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="50.1" customHeight="1">
@@ -4755,14 +4760,14 @@
         <v>41</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E51" s="27"/>
       <c r="F51" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="50.1" customHeight="1">
@@ -4770,22 +4775,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="50.1" customHeight="1">
@@ -4793,22 +4798,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="50.1" customHeight="1">
@@ -4816,22 +4821,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C54" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E54" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E54" s="27" t="s">
-        <v>92</v>
-      </c>
       <c r="F54" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="50.1" customHeight="1">
@@ -4839,22 +4844,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E55" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D55" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E55" s="27" t="s">
-        <v>102</v>
-      </c>
       <c r="F55" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="50.1" customHeight="1">
@@ -4862,22 +4867,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E56" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E56" s="27" t="s">
-        <v>238</v>
-      </c>
       <c r="F56" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="50.1" customHeight="1">
@@ -4885,22 +4890,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E57" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="E57" s="27" t="s">
-        <v>104</v>
-      </c>
       <c r="F57" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="50.1" customHeight="1">
@@ -4908,22 +4913,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>112</v>
-      </c>
       <c r="F58" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="50.1" customHeight="1">
@@ -4931,22 +4936,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E59" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E59" s="27" t="s">
-        <v>125</v>
-      </c>
       <c r="F59" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="50.1" customHeight="1">
@@ -4954,22 +4959,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C60" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E60" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E60" s="27" t="s">
-        <v>136</v>
-      </c>
       <c r="F60" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H60" s="1"/>
     </row>
@@ -4978,22 +4983,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C61" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E61" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E61" s="27" t="s">
-        <v>151</v>
-      </c>
       <c r="F61" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H61" s="1"/>
     </row>
@@ -5005,14 +5010,14 @@
         <v>41</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E62" s="27"/>
       <c r="F62" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H62" s="1"/>
     </row>
@@ -5024,14 +5029,14 @@
         <v>41</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E63" s="27"/>
       <c r="F63" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H63" s="1"/>
     </row>
@@ -5043,14 +5048,14 @@
         <v>41</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E64" s="27"/>
       <c r="F64" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H64" s="1"/>
     </row>
@@ -5062,17 +5067,17 @@
         <v>41</v>
       </c>
       <c r="C65" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="E65" s="27"/>
       <c r="F65" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H65" s="1"/>
     </row>
@@ -5081,22 +5086,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H66" s="1"/>
     </row>
@@ -5108,19 +5113,19 @@
         <v>7</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E67" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H67" s="1"/>
     </row>
@@ -5132,19 +5137,19 @@
         <v>7</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E68" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H68" s="1"/>
     </row>
@@ -5156,19 +5161,19 @@
         <v>7</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H69" s="1"/>
     </row>
@@ -5180,19 +5185,19 @@
         <v>7</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H70" s="1"/>
     </row>
@@ -5204,19 +5209,19 @@
         <v>7</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E71" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H71" s="1"/>
     </row>
@@ -5228,19 +5233,19 @@
         <v>41</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H72" s="1"/>
     </row>
@@ -5252,14 +5257,14 @@
         <v>41</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E73" s="27"/>
       <c r="F73" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H73" s="1"/>
     </row>
@@ -5271,14 +5276,14 @@
         <v>41</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E74" s="27"/>
       <c r="F74" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H74" s="1"/>
     </row>
@@ -5296,13 +5301,13 @@
         <v>13</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H75" s="1"/>
     </row>
@@ -5314,19 +5319,19 @@
         <v>7</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H76" s="1"/>
     </row>
@@ -5338,19 +5343,19 @@
         <v>7</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H77" s="7"/>
     </row>
@@ -5362,19 +5367,19 @@
         <v>7</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H78" s="7"/>
     </row>
@@ -5386,19 +5391,19 @@
         <v>7</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H79" s="7"/>
     </row>
@@ -5416,13 +5421,13 @@
         <v>20</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H80" s="7"/>
     </row>
@@ -5440,13 +5445,13 @@
         <v>29</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H81" s="7"/>
     </row>
@@ -5458,19 +5463,19 @@
         <v>7</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D82" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E82" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="E82" s="27" t="s">
-        <v>249</v>
-      </c>
       <c r="F82" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H82" s="7"/>
     </row>
@@ -5482,16 +5487,16 @@
         <v>41</v>
       </c>
       <c r="C83" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E83" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E83" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="F83" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H83" s="7"/>
     </row>
@@ -5503,14 +5508,14 @@
         <v>41</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E84" s="27"/>
       <c r="F84" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H84" s="7"/>
     </row>
@@ -5519,22 +5524,22 @@
         <v>84</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H85" s="7"/>
     </row>
@@ -5546,19 +5551,19 @@
         <v>7</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H86" s="7"/>
     </row>
@@ -5570,14 +5575,14 @@
         <v>41</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E87" s="27"/>
       <c r="F87" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H87" s="7"/>
     </row>
@@ -5589,16 +5594,16 @@
         <v>41</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H88" s="7"/>
     </row>
@@ -5607,22 +5612,22 @@
         <v>88</v>
       </c>
       <c r="B89" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C89" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E89" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="C89" s="28" t="s">
-        <v>399</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="E89" s="27" t="s">
-        <v>119</v>
-      </c>
       <c r="F89" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H89" s="7"/>
     </row>
@@ -5631,22 +5636,22 @@
         <v>89</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C90" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E90" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E90" s="27" t="s">
-        <v>398</v>
-      </c>
       <c r="F90" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H90" s="8"/>
     </row>
@@ -5658,19 +5663,19 @@
         <v>7</v>
       </c>
       <c r="C91" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="D91" s="27" t="s">
-        <v>222</v>
-      </c>
       <c r="E91" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H91" s="8"/>
     </row>
@@ -5682,16 +5687,16 @@
         <v>41</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G92" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H92" s="8"/>
     </row>
@@ -5703,16 +5708,16 @@
         <v>41</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H93" s="8"/>
     </row>
@@ -5730,13 +5735,13 @@
         <v>11</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H94" s="8"/>
     </row>
@@ -5754,13 +5759,13 @@
         <v>12</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H95" s="8"/>
     </row>
@@ -5772,19 +5777,19 @@
         <v>7</v>
       </c>
       <c r="C96" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D96" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D96" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="E96" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H96" s="8"/>
     </row>
@@ -5796,19 +5801,19 @@
         <v>41</v>
       </c>
       <c r="C97" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D97" s="6" t="s">
-        <v>197</v>
-      </c>
       <c r="E97" s="27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G97" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H97" s="8"/>
     </row>
@@ -5820,16 +5825,16 @@
         <v>41</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G98" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H98" s="8"/>
     </row>
@@ -5841,16 +5846,16 @@
         <v>41</v>
       </c>
       <c r="C99" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E99" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E99" s="27" t="s">
-        <v>59</v>
-      </c>
       <c r="F99" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H99" s="8"/>
     </row>
@@ -5859,22 +5864,22 @@
         <v>99</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H100" s="8"/>
     </row>
@@ -5883,22 +5888,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C101" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E101" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D101" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E101" s="27" t="s">
-        <v>121</v>
-      </c>
       <c r="F101" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H101" s="8"/>
     </row>
@@ -5907,22 +5912,22 @@
         <v>101</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H102" s="8"/>
     </row>
@@ -5931,22 +5936,22 @@
         <v>102</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="50.1" customHeight="1">
@@ -5957,19 +5962,19 @@
         <v>7</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H104" s="8"/>
     </row>
@@ -5987,13 +5992,13 @@
         <v>25</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H105" s="8"/>
     </row>
@@ -6005,19 +6010,19 @@
         <v>7</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H106" s="8"/>
     </row>
@@ -6029,19 +6034,19 @@
         <v>7</v>
       </c>
       <c r="C107" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="D107" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D107" s="6" t="s">
-        <v>247</v>
-      </c>
       <c r="E107" s="27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F107" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H107" s="8"/>
     </row>
@@ -6059,13 +6064,13 @@
         <v>34</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F108" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H108" s="8"/>
     </row>
@@ -6077,16 +6082,16 @@
         <v>41</v>
       </c>
       <c r="C109" s="28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E109" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="F109" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="F109" s="10" t="s">
-        <v>281</v>
-      </c>
       <c r="G109" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H109" s="8"/>
     </row>
@@ -6098,14 +6103,14 @@
         <v>41</v>
       </c>
       <c r="C110" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E110" s="27"/>
       <c r="F110" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H110" s="8"/>
     </row>
@@ -6114,22 +6119,22 @@
         <v>110</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C111" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H111" s="8"/>
     </row>
@@ -6138,22 +6143,22 @@
         <v>111</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C112" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E112" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E112" s="27" t="s">
-        <v>149</v>
-      </c>
       <c r="F112" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H112" s="9"/>
     </row>
@@ -6165,16 +6170,16 @@
         <v>41</v>
       </c>
       <c r="C113" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H113" s="9"/>
     </row>
@@ -6183,22 +6188,22 @@
         <v>113</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C114" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E114" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D114" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E114" s="27" t="s">
-        <v>117</v>
-      </c>
       <c r="F114" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="50.1" customHeight="1">
@@ -6206,22 +6211,22 @@
         <v>114</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C115" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E115" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E115" s="27" t="s">
-        <v>153</v>
-      </c>
       <c r="F115" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G115" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="50.1" customHeight="1">
@@ -6232,19 +6237,19 @@
         <v>41</v>
       </c>
       <c r="C116" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E116" s="27" t="s">
         <v>44</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G116" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="50.1" customHeight="1">
@@ -6255,16 +6260,16 @@
         <v>41</v>
       </c>
       <c r="C117" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E117" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="50.1" customHeight="1">
@@ -6275,14 +6280,14 @@
         <v>41</v>
       </c>
       <c r="C118" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E118" s="27"/>
       <c r="F118" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="50.1" customHeight="1">
@@ -6293,16 +6298,16 @@
         <v>41</v>
       </c>
       <c r="C119" s="28" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E119" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F119" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="50.1" customHeight="1">
@@ -6313,16 +6318,16 @@
         <v>41</v>
       </c>
       <c r="C120" s="28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E120" s="27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="50.1" customHeight="1">
@@ -6333,19 +6338,19 @@
         <v>7</v>
       </c>
       <c r="C121" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F121" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G121" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="50.1" customHeight="1">
@@ -6353,22 +6358,22 @@
         <v>121</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C122" s="28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E122" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F122" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G122" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="50.1" customHeight="1">
@@ -6376,22 +6381,22 @@
         <v>122</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C123" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E123" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D123" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E123" s="27" t="s">
-        <v>130</v>
-      </c>
       <c r="F123" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G123" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="50.1" customHeight="1">
@@ -6402,14 +6407,14 @@
         <v>41</v>
       </c>
       <c r="C124" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E124" s="27"/>
       <c r="F124" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="50.1" customHeight="1">
@@ -6417,22 +6422,22 @@
         <v>124</v>
       </c>
       <c r="B125" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C125" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C125" s="28" t="s">
-        <v>86</v>
-      </c>
       <c r="D125" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E125" s="27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F125" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="50.1" customHeight="1">
@@ -6440,22 +6445,22 @@
         <v>125</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C126" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D126" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E126" s="27" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F126" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="50.1" customHeight="1">
@@ -6463,22 +6468,22 @@
         <v>126</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C127" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E127" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D127" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E127" s="27" t="s">
-        <v>90</v>
-      </c>
       <c r="F127" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="50.1" customHeight="1">
@@ -6486,22 +6491,22 @@
         <v>127</v>
       </c>
       <c r="B128" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C128" s="28" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E128" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F128" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="50.1" customHeight="1">
@@ -6509,22 +6514,22 @@
         <v>128</v>
       </c>
       <c r="B129" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C129" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D129" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E129" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D129" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E129" s="27" t="s">
-        <v>100</v>
-      </c>
       <c r="F129" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="50.1" customHeight="1">
@@ -6532,22 +6537,22 @@
         <v>129</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C130" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E130" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E130" s="27" t="s">
-        <v>114</v>
-      </c>
       <c r="F130" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="50.1" customHeight="1">
@@ -6555,22 +6560,22 @@
         <v>130</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C131" s="28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E131" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F131" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="50.1" customHeight="1">
@@ -6578,22 +6583,22 @@
         <v>131</v>
       </c>
       <c r="B132" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C132" s="28" t="s">
+        <v>416</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E132" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="D132" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E132" s="27" t="s">
-        <v>418</v>
-      </c>
       <c r="F132" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G132" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="50.1" customHeight="1">
@@ -6604,19 +6609,19 @@
         <v>7</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D133" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E133" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="E133" s="27" t="s">
-        <v>212</v>
-      </c>
       <c r="F133" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G133" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="50.1" customHeight="1">
@@ -6627,19 +6632,19 @@
         <v>7</v>
       </c>
       <c r="C134" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E134" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G134" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="50.1" customHeight="1">
@@ -6650,16 +6655,16 @@
         <v>41</v>
       </c>
       <c r="C135" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E135" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G135" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="50.1" customHeight="1">
@@ -6670,16 +6675,16 @@
         <v>41</v>
       </c>
       <c r="C136" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E136" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F136" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G136" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="50.1" customHeight="1">
@@ -6690,16 +6695,16 @@
         <v>41</v>
       </c>
       <c r="C137" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E137" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F137" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="50.1" customHeight="1">
@@ -6710,14 +6715,14 @@
         <v>41</v>
       </c>
       <c r="C138" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E138" s="27"/>
       <c r="F138" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="50.1" customHeight="1">
@@ -6728,17 +6733,17 @@
         <v>41</v>
       </c>
       <c r="C139" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E139" s="27"/>
       <c r="F139" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G139" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="50.1" customHeight="1">
@@ -6746,22 +6751,22 @@
         <v>139</v>
       </c>
       <c r="B140" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C140" s="28" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D140" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E140" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="50.1" customHeight="1">
@@ -6769,22 +6774,22 @@
         <v>140</v>
       </c>
       <c r="B141" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C141" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D141" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E141" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D141" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E141" s="27" t="s">
-        <v>94</v>
-      </c>
       <c r="F141" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="50.1" customHeight="1">
@@ -6792,22 +6797,22 @@
         <v>141</v>
       </c>
       <c r="B142" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C142" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E142" s="27" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F142" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="50.1" customHeight="1">
@@ -6815,22 +6820,22 @@
         <v>142</v>
       </c>
       <c r="B143" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C143" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E143" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F143" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="50.1" customHeight="1">
@@ -6838,22 +6843,22 @@
         <v>143</v>
       </c>
       <c r="B144" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C144" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E144" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D144" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E144" s="27" t="s">
-        <v>107</v>
-      </c>
       <c r="F144" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="50.1" customHeight="1">
@@ -6861,22 +6866,22 @@
         <v>144</v>
       </c>
       <c r="B145" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C145" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E145" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G145" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="50.1" customHeight="1">
@@ -6884,22 +6889,22 @@
         <v>145</v>
       </c>
       <c r="B146" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C146" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E146" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="50.1" customHeight="1">
@@ -6907,22 +6912,22 @@
         <v>146</v>
       </c>
       <c r="B147" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C147" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E147" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="50.1" customHeight="1">
@@ -6933,19 +6938,19 @@
         <v>7</v>
       </c>
       <c r="C148" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D148" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="D148" s="6" t="s">
-        <v>210</v>
-      </c>
       <c r="E148" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F148" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G148" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="50.1" customHeight="1">
@@ -6956,19 +6961,19 @@
         <v>7</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E149" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F149" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G149" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="50.1" customHeight="1">
@@ -6979,19 +6984,19 @@
         <v>7</v>
       </c>
       <c r="C150" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E150" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F150" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G150" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="50.1" customHeight="1">
@@ -7002,19 +7007,19 @@
         <v>7</v>
       </c>
       <c r="C151" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E151" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F151" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G151" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -7056,7 +7061,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7073,45 +7078,45 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75">
       <c r="A2" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75">
       <c r="A3" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75">
       <c r="A4" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6" s="15"/>
     </row>
@@ -7129,37 +7134,37 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B12" s="15"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B14" s="15"/>
     </row>
@@ -7171,37 +7176,37 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B19" s="15"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B21" s="15"/>
     </row>
@@ -7288,7 +7293,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -7599,15 +7604,15 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="13">
         <v>27</v>
@@ -7615,7 +7620,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="13">
         <v>7</v>
@@ -7623,7 +7628,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" s="13">
         <v>7</v>
@@ -7631,18 +7636,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B5" s="13">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B6" s="13">
         <v>10</v>
@@ -7650,7 +7655,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B7" s="13">
         <v>33</v>
@@ -7658,7 +7663,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B8" s="13">
         <v>6</v>
@@ -7666,7 +7671,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B9" s="13">
         <v>6</v>
@@ -7682,18 +7687,18 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B11" s="13">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B12" s="13">
         <v>14</v>
@@ -7701,7 +7706,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B13" s="13">
         <v>51</v>
@@ -7709,7 +7714,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B14" s="13">
         <v>10</v>
@@ -7717,7 +7722,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B15" s="13">
         <v>11</v>
@@ -7725,18 +7730,18 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B16" s="13">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B17" s="13">
         <v>5</v>
@@ -7744,7 +7749,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B18" s="13">
         <v>5</v>
@@ -7752,7 +7757,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="13">
         <v>12</v>
@@ -7760,18 +7765,18 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B20" s="13">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B21" s="13">
         <v>39</v>
@@ -7779,18 +7784,18 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B22" s="13">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="13">
         <v>6</v>
@@ -7798,18 +7803,18 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B24" s="13">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B25" s="13">
         <v>11</v>
@@ -7817,7 +7822,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B26" s="13">
         <v>14</v>
@@ -7825,18 +7830,18 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B27" s="13">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B28" s="13">
         <v>150</v>
@@ -7852,7 +7857,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -7904,7 +7909,7 @@
     </row>
     <row r="3" spans="1:37">
       <c r="A3" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3">
         <f>E12*E14+G12*G14+I12*I14+K12*K14</f>
@@ -7923,7 +7928,7 @@
     </row>
     <row r="4" spans="1:37">
       <c r="A4" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B4">
         <f>(E16*E18+E16*E19)/2+ (G16*G18+G16*G19)/2+(I16*I18+I16*I19)/2+(K16*K18+K16*K19)/2</f>
@@ -7952,7 +7957,7 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5">
         <f>(E21*E23+E21*E24+ E21*E25)/3+ (G21*G23+G21*G24+G21*G25)/3+(I21*I23+I21*I24+I21*I25)/3+(K21*K23+K21*K24+K21*K25)/3+(M21*M23+M21*M24+M21*M25)/3</f>
@@ -7961,16 +7966,16 @@
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:37" ht="15.75" thickBot="1"/>
     <row r="11" spans="1:37">
       <c r="C11" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="35"/>
@@ -7984,31 +7989,31 @@
     </row>
     <row r="12" spans="1:37">
       <c r="C12" s="37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E12" s="23">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Deployment Testing","SuperGroup","Delivery Factors")</f>
         <v>7</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G12" s="23">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Integration of Software","SuperGroup","Delivery Factors")</f>
         <v>7</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I12" s="23">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Technology Tools","SuperGroup","Delivery Factors")</f>
         <v>3</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K12" s="24">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Trouble Shooting","SuperGroup","Delivery Factors")</f>
@@ -8019,22 +8024,22 @@
     </row>
     <row r="13" spans="1:37">
       <c r="C13" s="44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G13" s="42"/>
       <c r="H13" s="46" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I13" s="42"/>
       <c r="J13" s="42" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K13" s="43"/>
       <c r="L13" s="12"/>
@@ -8042,7 +8047,7 @@
     </row>
     <row r="14" spans="1:37" ht="15.75" thickBot="1">
       <c r="C14" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="40">
@@ -8065,10 +8070,10 @@
     </row>
     <row r="15" spans="1:37">
       <c r="C15" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="35"/>
@@ -8082,17 +8087,17 @@
     </row>
     <row r="16" spans="1:37">
       <c r="C16" s="39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E16" s="25">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Project Monitoring","SuperGroup","Implementation Factors")</f>
         <v>6</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G16" s="25">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Schedules/Deadlines","SuperGroup","Implementation Factors")</f>
@@ -8106,7 +8111,7 @@
         <v>5</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K16" s="26">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Workflow Communication","SuperGroup","Implementation Factors")</f>
@@ -8117,22 +8122,22 @@
     </row>
     <row r="17" spans="3:13">
       <c r="C17" s="39" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I17" s="25"/>
       <c r="J17" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K17" s="26"/>
       <c r="L17" s="12"/>
@@ -8140,7 +8145,7 @@
     </row>
     <row r="18" spans="3:13">
       <c r="C18" s="37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23">
@@ -8163,7 +8168,7 @@
     </row>
     <row r="19" spans="3:13" ht="15.75" thickBot="1">
       <c r="C19" s="38" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30">
@@ -8186,10 +8191,10 @@
     </row>
     <row r="20" spans="3:13">
       <c r="C20" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="35"/>
@@ -8203,38 +8208,38 @@
     </row>
     <row r="21" spans="3:13">
       <c r="C21" s="39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E21" s="25">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Contract Status","SuperGroup","Management Factors")</f>
         <v>10</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="25">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Management Assumptions","SuperGroup","Management Factors")</f>
         <v>11</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I21" s="25">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Project Expertise","SuperGroup","Management Factors")</f>
         <v>5</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K21" s="25">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Project Management Skills","SuperGroup","Management Factors")</f>
         <v>5</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M21" s="26">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Stakeholder Politics","SuperGroup","Management Factors")</f>
@@ -8243,32 +8248,32 @@
     </row>
     <row r="22" spans="3:13">
       <c r="C22" s="39" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M22" s="26"/>
     </row>
     <row r="23" spans="3:13">
       <c r="C23" s="32" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23">
@@ -8293,7 +8298,7 @@
     </row>
     <row r="24" spans="3:13">
       <c r="C24" s="32" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23">
@@ -8318,7 +8323,7 @@
     </row>
     <row r="25" spans="3:13" ht="15.75" thickBot="1">
       <c r="C25" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30">
@@ -8343,10 +8348,10 @@
     </row>
     <row r="26" spans="3:13">
       <c r="C26" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="35"/>
@@ -8360,24 +8365,24 @@
     </row>
     <row r="27" spans="3:13">
       <c r="C27" s="37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E27" s="23">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Project Complexity","SuperGroup","Planning Factors")</f>
         <v>6</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G27" s="23">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Project Objectives and Goals","SuperGroup","Planning Factors")</f>
         <v>11</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I27" s="24">
         <f>GETPIVOTDATA("SuperGroup",'Tag Count'!$A$1,"Code","Project Risk Analysis","SuperGroup","Planning Factors")</f>
@@ -8390,18 +8395,18 @@
     </row>
     <row r="28" spans="3:13">
       <c r="C28" s="44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E28" s="42"/>
       <c r="F28" s="42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G28" s="42"/>
       <c r="H28" s="42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I28" s="43"/>
       <c r="J28" s="12"/>
@@ -8411,7 +8416,7 @@
     </row>
     <row r="29" spans="3:13">
       <c r="C29" s="45" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23">
@@ -8432,7 +8437,7 @@
     </row>
     <row r="30" spans="3:13">
       <c r="C30" s="32" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23">
@@ -8453,7 +8458,7 @@
     </row>
     <row r="31" spans="3:13">
       <c r="C31" s="32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="23">
@@ -8474,7 +8479,7 @@
     </row>
     <row r="32" spans="3:13" ht="15.75" thickBot="1">
       <c r="C32" s="38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30">

</xml_diff>